<commit_message>
database update, moves in infobox
</commit_message>
<xml_diff>
--- a/app/baza.xlsx
+++ b/app/baza.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\R\memoryGame\app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8912BCA-410C-45FA-83BD-82055DD5E26B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ECEECAA-AB49-4409-86C0-DFA0C97E883B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{C4E2EA9A-07B3-471B-BD5D-C42FADB100C1}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="63">
   <si>
     <t>poziom</t>
   </si>
@@ -115,9 +115,6 @@
     <t>kwartyl górny</t>
   </si>
   <si>
-    <t>średnia</t>
-  </si>
-  <si>
     <t>średnia wartość cechy</t>
   </si>
   <si>
@@ -127,12 +124,6 @@
     <t>brak interpretacji</t>
   </si>
   <si>
-    <t>współczynnik zmienności</t>
-  </si>
-  <si>
-    <t>zróżnicowanie wyrażone w procentach</t>
-  </si>
-  <si>
     <t>skośność</t>
   </si>
   <si>
@@ -145,10 +136,91 @@
     <t>czy rozkład cechy jest normalny, spłaszczony lub wysmukły</t>
   </si>
   <si>
-    <t>50% jednostek posiada wartości poniżej mediany a 50% powyżej</t>
-  </si>
-  <si>
-    <t>75% jednostek posiada wartości poniżej mediany a 25% powyżej</t>
+    <t>x_i</t>
+  </si>
+  <si>
+    <t>wariant cechy</t>
+  </si>
+  <si>
+    <t>x_sr</t>
+  </si>
+  <si>
+    <t>średnia arytmetyczna</t>
+  </si>
+  <si>
+    <t>typowy obszar zmienności</t>
+  </si>
+  <si>
+    <t>reguła trzech sigm</t>
+  </si>
+  <si>
+    <t>w odległości 3 odchyleń standardowych od średniej jest 99,7% obserwacji</t>
+  </si>
+  <si>
+    <t>średnia +/- odchylenie standardowe - 68,3% obserwacji</t>
+  </si>
+  <si>
+    <t>zróżnicowanie cechy wyrażone w procentach</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>kwartyl dolny</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>odchylenie ćwiartkowe</t>
+  </si>
+  <si>
+    <t>Vq</t>
+  </si>
+  <si>
+    <t>pozycyjny współczynnik zmienności</t>
+  </si>
+  <si>
+    <t>Aq</t>
+  </si>
+  <si>
+    <t>pozycyjny współczynnik asymetrii</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>rozstęp</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>dominanta</t>
+  </si>
+  <si>
+    <t>50% obserwacji posiada wartości niższe lub równe medianie, a 50% wyższe lub równe</t>
+  </si>
+  <si>
+    <t>75% obserwacji posiada wartości niższe lub równe Q3, a 25% wyższe lub równe</t>
+  </si>
+  <si>
+    <t>25% obserwacji posiada wartości niższe lub równe Q1, a 75% wyższe lub równe</t>
+  </si>
+  <si>
+    <t>przeciętne odchylenie od mediany u środkowych 50% obserwacji</t>
+  </si>
+  <si>
+    <t>różnica pomiędzy wartością maksymalną i minimalną</t>
+  </si>
+  <si>
+    <t>najczęściej występująca wartość</t>
+  </si>
+  <si>
+    <t>kwartyl górny (Q3)</t>
+  </si>
+  <si>
+    <t>kwartyl dolny (Q1)</t>
   </si>
 </sst>
 </file>
@@ -615,17 +687,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3F4DD1C-8133-44DB-8F91-9C2F5772A1A0}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="75.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="78.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -710,10 +782,10 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -721,10 +793,10 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -732,10 +804,10 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" t="s">
         <v>27</v>
-      </c>
-      <c r="C10" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -746,7 +818,7 @@
         <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -757,7 +829,7 @@
         <v>16</v>
       </c>
       <c r="C12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -765,10 +837,10 @@
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="C13" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -776,10 +848,10 @@
         <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C14" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -787,10 +859,10 @@
         <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C15" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -798,10 +870,10 @@
         <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="C16" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -809,10 +881,186 @@
         <v>2</v>
       </c>
       <c r="B17" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>3</v>
+      </c>
+      <c r="B18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>3</v>
+      </c>
+      <c r="B19" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" t="s">
         <v>26</v>
       </c>
-      <c r="C17" t="s">
-        <v>38</v>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>3</v>
+      </c>
+      <c r="B20" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>3</v>
+      </c>
+      <c r="B21" t="s">
+        <v>45</v>
+      </c>
+      <c r="C21" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>3</v>
+      </c>
+      <c r="B22" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>3</v>
+      </c>
+      <c r="B23" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>3</v>
+      </c>
+      <c r="B24" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>3</v>
+      </c>
+      <c r="B25" t="s">
+        <v>53</v>
+      </c>
+      <c r="C25" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>4</v>
+      </c>
+      <c r="B26" t="s">
+        <v>24</v>
+      </c>
+      <c r="C26" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>4</v>
+      </c>
+      <c r="B27" t="s">
+        <v>61</v>
+      </c>
+      <c r="C27" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>4</v>
+      </c>
+      <c r="B28" t="s">
+        <v>62</v>
+      </c>
+      <c r="C28" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>4</v>
+      </c>
+      <c r="B29" t="s">
+        <v>46</v>
+      </c>
+      <c r="C29" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>4</v>
+      </c>
+      <c r="B30" t="s">
+        <v>48</v>
+      </c>
+      <c r="C30" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>4</v>
+      </c>
+      <c r="B31" t="s">
+        <v>50</v>
+      </c>
+      <c r="C31" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>4</v>
+      </c>
+      <c r="B32" t="s">
+        <v>52</v>
+      </c>
+      <c r="C32" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>4</v>
+      </c>
+      <c r="B33" t="s">
+        <v>54</v>
+      </c>
+      <c r="C33" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
dodanie pytań z korelacji i regresji
</commit_message>
<xml_diff>
--- a/app/baza.xlsx
+++ b/app/baza.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\R\memoryGame\app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FA0EFF2-D91C-400B-9757-265ED2E8BCD0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BADB3062-D559-411D-BB27-BF49E7CD27CA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{C4E2EA9A-07B3-471B-BD5D-C42FADB100C1}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="125">
   <si>
     <t>poziom</t>
   </si>
@@ -275,6 +275,138 @@
   </si>
   <si>
     <t>czy rozkład cechy jest symetryczny, lewo lub prawostronnie asymetryczny</t>
+  </si>
+  <si>
+    <t>pomiędzy cechami jakościowymi występuje słaba zależność</t>
+  </si>
+  <si>
+    <t>pomiędzy cechami jakościowymi występuje silna zależność</t>
+  </si>
+  <si>
+    <t>0 &lt; V &lt; 0,3</t>
+  </si>
+  <si>
+    <t>0,5 &lt; V &lt; 1</t>
+  </si>
+  <si>
+    <t>0,3 &lt; V &lt; 0,5</t>
+  </si>
+  <si>
+    <t>pomiędzy cechami jakościowymi występuje umiarkowana zależność</t>
+  </si>
+  <si>
+    <t>r = 1</t>
+  </si>
+  <si>
+    <t>pomiędzy cechami ilościowymi występuje dodatnia korelacja doskonała</t>
+  </si>
+  <si>
+    <t>r = -1</t>
+  </si>
+  <si>
+    <t>pomiędzy cechami ilościowymi występuje ujemna korelacja doskonała</t>
+  </si>
+  <si>
+    <t>r = 0</t>
+  </si>
+  <si>
+    <t>pomiędzy cechami ilościowymi nie występuje zależność</t>
+  </si>
+  <si>
+    <t>0 &lt; r &lt; 1</t>
+  </si>
+  <si>
+    <t>pomiędzy cechami ilościowymi występuje dodatnia (słaba/umiarkowana/silna) korelacja niedoskonała</t>
+  </si>
+  <si>
+    <t>-1 &lt; r &lt; 0</t>
+  </si>
+  <si>
+    <t>pomiędzy cechami ilościowymi występuje ujemna (słaba/umiarkowana/silna) korelacja niedoskonała</t>
+  </si>
+  <si>
+    <t>a1</t>
+  </si>
+  <si>
+    <t>a0</t>
+  </si>
+  <si>
+    <t>Su</t>
+  </si>
+  <si>
+    <t>R^2</t>
+  </si>
+  <si>
+    <t>fi^2</t>
+  </si>
+  <si>
+    <t>SKR</t>
+  </si>
+  <si>
+    <t>Vu</t>
+  </si>
+  <si>
+    <t>współczynnik kierunkowy</t>
+  </si>
+  <si>
+    <t>wyraz wolny</t>
+  </si>
+  <si>
+    <t>odchylenie standardowe składnika resztowego</t>
+  </si>
+  <si>
+    <t>współczynnik determinacji</t>
+  </si>
+  <si>
+    <t xml:space="preserve">współczynnik zbieżności </t>
+  </si>
+  <si>
+    <t>suma kwadratów reszt</t>
+  </si>
+  <si>
+    <t>współczynnik zmienności resztowej</t>
+  </si>
+  <si>
+    <t>Su^T</t>
+  </si>
+  <si>
+    <t>błąd prognozy</t>
+  </si>
+  <si>
+    <t>współczynnik kierunkowy regresji</t>
+  </si>
+  <si>
+    <t>przeciętna zmiana Y w przypadku wzrostu X o jednostkę</t>
+  </si>
+  <si>
+    <t>wyraz wolny regresji</t>
+  </si>
+  <si>
+    <t>teoretyczny poziom Y jeśli X = 0</t>
+  </si>
+  <si>
+    <t>współczynnik kierunkowy trendu</t>
+  </si>
+  <si>
+    <t>przeciętna zmiana Y z okresu na okres</t>
+  </si>
+  <si>
+    <t>wyraz wolny trendu</t>
+  </si>
+  <si>
+    <t>teoretyczny poziom Y w okresie poprzedzającym analizę</t>
+  </si>
+  <si>
+    <t>przeciętne odchylenie wartości empirycznych od teoretycznych</t>
+  </si>
+  <si>
+    <t>odsetek wahań losowych w średnim poziomie Y</t>
+  </si>
+  <si>
+    <t>procent wariancji (zmienności) zmiennej Y wyjaśniony przez model</t>
+  </si>
+  <si>
+    <t>procent wariancji (zmienności) zmiennej Y nie wyjaśniony przez model</t>
   </si>
 </sst>
 </file>
@@ -311,8 +443,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -741,16 +874,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3F4DD1C-8133-44DB-8F91-9C2F5772A1A0}">
-  <dimension ref="A1:C41"/>
+  <dimension ref="A1:C65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="A66" sqref="A66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="102.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -1206,6 +1339,270 @@
         <v>76</v>
       </c>
     </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>6</v>
+      </c>
+      <c r="B42" t="s">
+        <v>83</v>
+      </c>
+      <c r="C42" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>6</v>
+      </c>
+      <c r="B43" t="s">
+        <v>84</v>
+      </c>
+      <c r="C43" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>6</v>
+      </c>
+      <c r="B44" t="s">
+        <v>85</v>
+      </c>
+      <c r="C44" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>6</v>
+      </c>
+      <c r="B45" t="s">
+        <v>87</v>
+      </c>
+      <c r="C45" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>6</v>
+      </c>
+      <c r="B46" t="s">
+        <v>89</v>
+      </c>
+      <c r="C46" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>6</v>
+      </c>
+      <c r="B47" t="s">
+        <v>91</v>
+      </c>
+      <c r="C47" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>6</v>
+      </c>
+      <c r="B48" t="s">
+        <v>93</v>
+      </c>
+      <c r="C48" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>6</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C49" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>7</v>
+      </c>
+      <c r="B50" t="s">
+        <v>97</v>
+      </c>
+      <c r="C50" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>7</v>
+      </c>
+      <c r="B51" t="s">
+        <v>98</v>
+      </c>
+      <c r="C51" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>7</v>
+      </c>
+      <c r="B52" t="s">
+        <v>99</v>
+      </c>
+      <c r="C52" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>7</v>
+      </c>
+      <c r="B53" t="s">
+        <v>100</v>
+      </c>
+      <c r="C53" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>7</v>
+      </c>
+      <c r="B54" t="s">
+        <v>101</v>
+      </c>
+      <c r="C54" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>7</v>
+      </c>
+      <c r="B55" t="s">
+        <v>102</v>
+      </c>
+      <c r="C55" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>7</v>
+      </c>
+      <c r="B56" t="s">
+        <v>103</v>
+      </c>
+      <c r="C56" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>7</v>
+      </c>
+      <c r="B57" t="s">
+        <v>111</v>
+      </c>
+      <c r="C57" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>8</v>
+      </c>
+      <c r="B58" t="s">
+        <v>113</v>
+      </c>
+      <c r="C58" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>8</v>
+      </c>
+      <c r="B59" t="s">
+        <v>115</v>
+      </c>
+      <c r="C59" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>8</v>
+      </c>
+      <c r="B60" t="s">
+        <v>117</v>
+      </c>
+      <c r="C60" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>8</v>
+      </c>
+      <c r="B61" t="s">
+        <v>119</v>
+      </c>
+      <c r="C61" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>8</v>
+      </c>
+      <c r="B62" t="s">
+        <v>106</v>
+      </c>
+      <c r="C62" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>8</v>
+      </c>
+      <c r="B63" t="s">
+        <v>107</v>
+      </c>
+      <c r="C63" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>8</v>
+      </c>
+      <c r="B64" t="s">
+        <v>108</v>
+      </c>
+      <c r="C64" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>8</v>
+      </c>
+      <c r="B65" t="s">
+        <v>110</v>
+      </c>
+      <c r="C65" t="s">
+        <v>122</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>